<commit_message>
Chanched and cleaned stocks code
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="АВТО" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="59">
   <si>
     <t xml:space="preserve">Общий V </t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>№</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Менеджер </t>
   </si>
   <si>
     <t>Дата</t>
@@ -718,11 +715,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -785,7 +782,7 @@
       </c>
       <c r="U1" s="15"/>
       <c r="V1" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W1" s="12" t="s">
         <v>3</v>
@@ -822,18 +819,18 @@
       </c>
       <c r="S2" s="17">
         <f ca="1">TODAY()</f>
-        <v>45188</v>
+        <v>45189</v>
       </c>
       <c r="T2" s="17">
         <v>45047</v>
       </c>
       <c r="U2" s="15">
         <f ca="1">S2-T2</f>
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="V2" s="12">
         <f ca="1">(R2-Q2)*U2</f>
-        <v>141000</v>
+        <v>142000</v>
       </c>
       <c r="W2" s="18">
         <f ca="1">Q2/R2</f>
@@ -849,73 +846,73 @@
         <v>4</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="I3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="K3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="M3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="N3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="23" t="s">
+      <c r="O3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="23" t="s">
+      <c r="P3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="Q3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="R3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="S3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="T3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="23" t="s">
+      <c r="U3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="V3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="23" t="s">
+      <c r="W3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="23" t="s">
+      <c r="X3" s="23" t="s">
         <v>26</v>
-      </c>
-      <c r="X3" s="23" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -26851,7 +26848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -26863,210 +26860,210 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="28" t="s">
+      <c r="B16" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
-        <v>33</v>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>44</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>55</v>
+      <c r="B17" s="28" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
-        <v>34</v>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>45</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>55</v>
+      <c r="B18" s="28" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
-        <v>35</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>46</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>59</v>
+      <c r="B19" s="28" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
-        <v>36</v>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>48</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>59</v>
+      <c r="B20" s="28" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
-        <v>37</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
+        <v>47</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>59</v>
+      <c r="B21" s="28" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
-        <v>38</v>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>49</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="B22" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="28" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>57</v>
+      <c r="B23" s="28" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="28" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>57</v>
+      <c r="B24" s="28" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="28" t="s">
-        <v>57</v>
+      <c r="B25" s="28" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
-        <v>54</v>
-      </c>
       <c r="B26" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -27087,762 +27084,762 @@
   <sheetData>
     <row r="1" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E2" t="s">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E3" t="s">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E69" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E71" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E78" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E80" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E82" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E84" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E85" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E86" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E87" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E88" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E89" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E90" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E91" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E92" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E93" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E94" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E96" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E97" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E98" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E99" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E102" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E104" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E105" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E107" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E108" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E109" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E110" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E111" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E112" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E113" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E114" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E115" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E116" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E117" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E118" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E119" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E120" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E121" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E4" t="s">
-        <v>30</v>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E122" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E5" t="s">
-        <v>41</v>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E123" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E6" t="s">
-        <v>30</v>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E124" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E7" t="s">
-        <v>41</v>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E125" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E8" t="s">
-        <v>30</v>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E126" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E9" t="s">
-        <v>30</v>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E127" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E128" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E129" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E15" t="s">
-        <v>40</v>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E130" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="16" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
-        <v>30</v>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E131" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E22" t="s">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E132" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E23" t="s">
-        <v>33</v>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E133" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E31" t="s">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E134" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E32" t="s">
-        <v>48</v>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E135" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E51" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E53" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E54" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E56" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E57" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E59" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E61" t="s">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E136" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E62" t="s">
-        <v>34</v>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E137" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E63" t="s">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E138" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E64" t="s">
-        <v>42</v>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E139" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E65" t="s">
-        <v>34</v>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E140" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E66" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E67" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E68" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E69" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E70" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E72" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E74" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E75" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E77" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E78" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E79" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E80" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E81" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E82" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E83" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E84" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E85" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E86" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E87" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E88" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E89" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E90" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E91" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E92" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E93" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E94" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E95" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E96" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E97" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E98" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E99" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E100" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E101" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E102" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E103" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E104" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E105" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E106" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E107" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E108" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E109" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E110" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E111" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E112" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E113" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E114" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E115" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E116" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E117" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E118" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E119" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E120" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E121" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E122" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E123" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E124" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E125" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E126" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E127" t="s">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E141" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E128" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E129" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E130" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E131" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E132" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E133" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E134" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E135" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E136" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E137" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E138" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E139" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E140" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E141" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="142" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E142" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E143" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="144" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E144" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E145" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E146" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="148" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E148" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="149" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E149" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E150" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="151" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E151" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="152" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E152" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>